<commit_message>
Auto-committed on 2022/08/24 週三 11:32:13.60
</commit_message>
<xml_diff>
--- a/Program/Other/一年內新貸件扣款失敗表-底稿.xlsx
+++ b/Program/Other/一年內新貸件扣款失敗表-底稿.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A48CAA4-94D0-44F7-A22E-C9A8245A8461}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580"/>
   </bookViews>
   <sheets>
     <sheet name="LAW7U1Pqp" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Database">LAW7U1Pqp!$A$1:$I$1</definedName>
+    <definedName name="_xlnm.Database">LAW7U1Pqp!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>戶名</t>
   </si>
@@ -52,11 +51,15 @@
   <si>
     <t>撥款日</t>
   </si>
+  <si>
+    <t>撥款</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -816,23 +819,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -868,23 +854,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1060,28 +1029,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="26.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.81640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1092,24 +1062,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>